<commit_message>
Status and queries for the week
* Updated status and follow up queries for the next week.
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthik\OneDrive\ananth\5th sem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400A138-FFBF-421D-B78E-49C83D7E7BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D414386B-C04A-4ED7-80C2-A4666B2B5C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -136,6 +136,15 @@
 4) How does "isDefined" function work?</t>
   </si>
   <si>
+    <t xml:space="preserve">1) Should validity of expression be checked for eg: how would ((2&lt;3)&lt;5) be evaluated?. </t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Expression evaluation</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1) Evaluate </t>
     </r>
@@ -244,17 +253,12 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Should validity of expression be checked for eg: how would ((2&lt;3)&lt;5) be evaluated?. </t>
-  </si>
-  <si>
-    <t>Implementation</t>
-  </si>
-  <si>
-    <t>Expression evaluation</t>
+3) The incoming JSON file is assumed to be valid as checks on validity of each dataType and returnType would feel too large
+4) "isDefined" function checks a resulting value of expression is not null, thereby testing the validty of the expression </t>
+    </r>
+  </si>
+  <si>
+    <t>1) The incoming JSON file is assumed to be valid as checks on validity of each dataType and returnType would feel too large</t>
   </si>
   <si>
     <r>
@@ -281,15 +285,87 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> etc 
-3) Unit tests written for validation purposes</t>
-    </r>
+3) Unit tests written for the same</t>
+    </r>
+  </si>
+  <si>
+    <t>1) isDefined function tests are written only for certain functions of `exp` type. Should 
+testExpr = {  'name': 'isDefined',
+        'data': [{'dType': 'number', 'str': '5'}};
+return a `false` ?</t>
+  </si>
+  <si>
+    <t>1) It comes under Survey Item Components ask back after Survey Item Component implementation</t>
+  </si>
+  <si>
+    <r>
+      <t>1) Queries related to Item Component implementation (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/influenzanet/survey-engine.dart/blob/development/documents/QandA.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/influenzanet/survey-engine.ts/wiki/Components-of-a-survey-item#components-of-a-survey-item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for documentation overview</t>
+    </r>
+  </si>
+  <si>
+    <t>Expression evaluation and Component study</t>
+  </si>
+  <si>
+    <t>1) Expression evaluation for combination of operators
+2) Further changes to expression evaluation after Q &amp; A 
+3) Identifying the next tasks
+4) Creation of query document in md (https://github.com/influenzanet/survey-engine.dart/blob/development/documents/QandA.md)
+5) Implementation of LocalisedMediaObject
+6) Implementation of DisplayComponent started</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,13 +381,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -323,10 +411,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -337,8 +426,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -387,8 +480,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D4" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D4" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D5" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -405,8 +498,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A8CD2E07-0777-4479-9697-C502B276A704}" name="Table8" displayName="Table8" ref="A1:C4" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C4" xr:uid="{6FF9E1DD-7A10-4235-8596-80FC9E7EFAB3}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A8CD2E07-0777-4479-9697-C502B276A704}" name="Table8" displayName="Table8" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C6" xr:uid="{6FF9E1DD-7A10-4235-8596-80FC9E7EFAB3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -717,22 +810,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.29296875" customWidth="1"/>
-    <col min="2" max="2" width="23.1171875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="60.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.29296875" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43868</v>
       </c>
@@ -760,7 +853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43873</v>
       </c>
@@ -774,18 +867,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>43888</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -802,17 +909,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1171875" customWidth="1"/>
-    <col min="2" max="2" width="58.87890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.41015625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -823,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43873</v>
       </c>
@@ -834,7 +941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43879</v>
       </c>
@@ -842,19 +949,43 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.5"/>
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>43884</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>43885</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q and As updated for survey item componentcreation
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthik\OneDrive\ananth\5th sem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D414386B-C04A-4ED7-80C2-A4666B2B5C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC19F09-74BF-4536-88AA-96B7EE8F3198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -360,12 +360,47 @@
 5) Implementation of LocalisedMediaObject
 6) Implementation of DisplayComponent started</t>
   </si>
+  <si>
+    <t>Item Component creation and Survey ItemComponent study</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Created ItemComponent classes and subclasses based on UML feedback.
+2) Using a concept of `factory` constructors inheritance through interfaces implementation taken care of.
+3) Initial outline questions on front-end/backend evaluation and plugin package automation.
+4) Updated Q and A markdown file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To do:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Complete Surevy Item Components outline next and start engine implementation
+2) Create a wiki on all learnings. A small dump is also fine</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +419,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,8 +523,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D5" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D7" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D7" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -810,22 +853,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.29296875" customWidth="1"/>
+    <col min="2" max="2" width="23.1171875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.29296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>43868</v>
       </c>
@@ -853,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>43873</v>
       </c>
@@ -867,7 +910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -881,7 +924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>43888</v>
       </c>
@@ -894,6 +937,26 @@
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="6" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
+      <c r="A6" s="3">
+        <v>43896</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -912,14 +975,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1171875" customWidth="1"/>
+    <col min="2" max="2" width="58.87890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -930,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>43873</v>
       </c>
@@ -941,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="86" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>43879</v>
       </c>
@@ -952,7 +1015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -963,7 +1026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>43884</v>
       </c>
@@ -974,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>43885</v>
       </c>
@@ -985,7 +1048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Survey Single Item object creation tested
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC19F09-74BF-4536-88AA-96B7EE8F3198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBED72FB-21AE-4E80-B247-A7919F424F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Updated Q&A and status
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBED72FB-21AE-4E80-B247-A7919F424F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCCBC5D-A3FD-4D75-8188-EF38EB4B9176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -364,6 +364,9 @@
     <t>Item Component creation and Survey ItemComponent study</t>
   </si>
   <si>
+    <t>SurveyComponent implementation</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1) Created ItemComponent classes and subclasses based on UML feedback.
 2) Using a concept of `factory` constructors inheritance through interfaces implementation taken care of.
@@ -391,9 +394,17 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-1) Complete Surevy Item Components outline next and start engine implementation
+1) Complete Survey Item Components outline next and start engine implementation
 2) Create a wiki on all learnings. A small dump is also fine</t>
     </r>
+  </si>
+  <si>
+    <t>1) Implemented and tested SurveyComponent outline classes
+2) Implemented SurveyResponseItem outline classes completing ouline of all respective class models in the Survey
+3) Studied expression-eval, engine.ts and made notes of doubts
+4) resolveContent in LocalisedObject expression implemented internally during the object creation
+5) SelectionMethod implemented for a dummy map of array items
+6) Created an issue for a `wiki` page. Will be updating in due course of `engine` development</t>
   </si>
 </sst>
 </file>
@@ -855,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -949,14 +960,22 @@
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="129" x14ac:dyDescent="0.5">
+      <c r="A7" s="3">
+        <v>43902</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Status and queries updated for next session
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E632C17F-923E-4D7C-98A5-8734F25BE661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68153F62-6E63-49CB-AB01-AB8F9D23A901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -420,6 +420,11 @@
 5) selection method and random distribution expressions implemented will be worked again later in due course after some more discussions
 6) Expression Evaluation `wiki` implemented
 7) TO DO: initResponseObject-&gt;constructor-&gt;findResponseItem-&gt;setTimestampFor-&gt;addRenderedItem</t>
+  </si>
+  <si>
+    <t>1) Discussion on upcoming queries
+2) Wrote a few flowcharts for surveyEngine like constructor,setTimestampFor,addRenderedItem and will be changed after some reviews
+3) Implemented `setTimeStampFor` function and tests</t>
   </si>
 </sst>
 </file>
@@ -549,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D8" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D8" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D9" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D9" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -879,22 +884,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.29296875" customWidth="1"/>
-    <col min="2" max="2" width="23.1171875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="60.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.29296875" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43868</v>
       </c>
@@ -922,7 +927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43873</v>
       </c>
@@ -936,7 +941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -950,7 +955,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43888</v>
       </c>
@@ -964,7 +969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43896</v>
       </c>
@@ -978,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="129" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43902</v>
       </c>
@@ -992,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="200.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>43915</v>
       </c>
@@ -1004,6 +1009,20 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>43916</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1023,14 +1042,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1171875" customWidth="1"/>
-    <col min="2" max="2" width="58.87890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.41015625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43873</v>
       </c>
@@ -1052,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="86" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43879</v>
       </c>
@@ -1063,7 +1082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -1074,7 +1093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43884</v>
       </c>
@@ -1085,7 +1104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43885</v>
       </c>
@@ -1096,7 +1115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Status and queries updated
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68153F62-6E63-49CB-AB01-AB8F9D23A901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8C5502-EBC4-4FC6-8BF1-CCFB8E139F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -425,6 +425,26 @@
     <t>1) Discussion on upcoming queries
 2) Wrote a few flowcharts for surveyEngine like constructor,setTimestampFor,addRenderedItem and will be changed after some reviews
 3) Implemented `setTimeStampFor` function and tests</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Flowchart creation and queries</t>
+  </si>
+  <si>
+    <t>1) Status and test cases shown
+2) Flowchart presented -- review opinion rework on flowchart and reove pseudo code from flowchart
+3) Hierarchy present for groups and single item keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Studied findResponse, Rendered Item
+2) Watched the control flow of init objects and deduced an algorithm thereby translating the constructor creation of Survey Engine
+3) Every ItemGroupComponent every single survey Item and every response Item is created as well as resolved (excluding rerender functions and expressions using rerender objects) in a sequential order
+4) Optimised the algorithm for fewer checks and wrote utility functions like getRootKey, removeNullparams etc for better clean code concepts as well as improving readability.
+5) Fixed major bugs relating to itemgroup coponent resolution and rendering Survey Group Component items and few others relating to validations, parts resolution etc
+6) Flowcharts rewritten with an abstract view by not including pseudocde until the reordering/rerendering of functions
+7) Updated query sheet and informed about freezing model==0.4.9 for now. The version will be implemeneted and tested then upcoming changes will be rendered appropriately </t>
   </si>
 </sst>
 </file>
@@ -554,8 +574,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D9" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D9" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D11" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D11" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -884,22 +904,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.29296875" customWidth="1"/>
+    <col min="2" max="2" width="23.1171875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.29296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>43868</v>
       </c>
@@ -927,7 +947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>43873</v>
       </c>
@@ -941,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -955,7 +975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>43888</v>
       </c>
@@ -969,7 +989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>43896</v>
       </c>
@@ -983,7 +1003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="129" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>43902</v>
       </c>
@@ -997,7 +1017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="200.7" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>43915</v>
       </c>
@@ -1011,7 +1031,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>43916</v>
       </c>
@@ -1023,6 +1043,34 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="3">
+        <v>43923</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="243.7" x14ac:dyDescent="0.5">
+      <c r="A11" s="3">
+        <v>43930</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1042,14 +1090,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1171875" customWidth="1"/>
+    <col min="2" max="2" width="58.87890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>43873</v>
       </c>
@@ -1071,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="86" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>43879</v>
       </c>
@@ -1082,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>43880</v>
       </c>
@@ -1093,7 +1141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>43884</v>
       </c>
@@ -1104,7 +1152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>43885</v>
       </c>
@@ -1115,7 +1163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tested public access methods
* Get response item in a list is tested
* Getting a rendered survey is tested
* Bug fix: Timestamp punched on every group item render during
initialisation
* Status updated
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5242927-DECA-42C8-A7E8-77AFF411847F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D162EF8-8562-4CF9-82CF-5CD1AC9E6B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -504,12 +504,13 @@
     </r>
   </si>
   <si>
+    <t>SurveyEngineCore Implementation and flowchart creation</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) initRenderedGroup and initSurveyresponseObjects completed. i.e the survey-engine parses conditions, evalConditions and renders the first set of Responses along with items and components in the initial step
 2) Implemented `sequential` in selection methods to make testing easy. The survey group items are picked randomly by default and was a harder to compare the structure with test objects so `sequential` is used as a workaroud default for now
-3) Came up with 5 theme names for the Master thesis topic  </t>
-  </si>
-  <si>
-    <t>SurveyEngineCore Implementation and flowchart creation</t>
+3) Came up with 5 theme names for the Master thesis topic  
+4) Public methods for getting a rendered survey and getting responses in flat tree done </t>
   </si>
 </sst>
 </file>
@@ -972,7 +973,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1146,13 +1147,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="143.35" x14ac:dyDescent="0.5">
       <c r="A13" s="3">
         <v>43944</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated status and query sheet
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D162EF8-8562-4CF9-82CF-5CD1AC9E6B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CF8FE1-3B8B-4286-8F7A-6C1E7E3088AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -511,6 +511,34 @@
 2) Implemented `sequential` in selection methods to make testing easy. The survey group items are picked randomly by default and was a harder to compare the structure with test objects so `sequential` is used as a workaroud default for now
 3) Came up with 5 theme names for the Master thesis topic  
 4) Public methods for getting a rendered survey and getting responses in flat tree done </t>
+  </si>
+  <si>
+    <t>Analysis, implementation and documentation</t>
+  </si>
+  <si>
+    <t>Expression Evaluation</t>
+  </si>
+  <si>
+    <r>
+      <t>1) Studied setResponseItem and started reRender studies
+2) On careful analysis realised that expression evaluation needs to be completed for rerendering. Without a valid getResponses a setResponse would make not much sense
+3) Studied all Array,Object and tree expressions.
+4) Created a wiki for the same expressions
+5) Implemented all the expressions and tested it in various scenarios. Testing can be improved.
+6) Queries updated
+7) Thesis topic name finalised as "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Analysis of the survey model and implementation of a survey engine for parsing survey components of the Influenzanet project on a smartphone screen: A Dart library for developing cross-platform flutter applications"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -640,8 +668,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D13" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D13" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D14" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D14" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -970,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1165,6 +1193,20 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="186.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="3">
+        <v>43951</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing set resposes with typescript logic
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5085E-D98D-47C7-B156-14E0A87A9203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5F765F-609F-4639-B2E8-712B36EBB692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -539,6 +539,17 @@
       </rPr>
       <t>Analysis of the survey model and implementation of a survey engine for parsing survey components of the Influenzanet project on a smartphone screen: A Dart library for developing cross-platform flutter applications"</t>
     </r>
+  </si>
+  <si>
+    <t>Analysis, implementation , documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) More study on rerender
+2) Model analysis and testing on SurveyItems from other models and web client.
+3) Fixed more bugs from new test surveys and also found issues with model diagrams like differing data types for components in ItemGroupComponent, also missing '?' in ResponseItem.value,dtype etc. Reported such non-mandatory items in slack.
+4) Revamped model and test cases with non-mandatory items, added new roles etc.
+5) Documentation of an goal/abstract sheet for the thesis 
+6) Prepped a JSON diff for the same survey item questions to discuss in meetings  </t>
   </si>
 </sst>
 </file>
@@ -668,8 +679,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D14" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D14" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D15" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D15" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -998,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1207,6 +1218,20 @@
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="172" x14ac:dyDescent="0.5">
+      <c r="A15" s="3">
+        <v>43958</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Status and query sheet update for syncup
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637019CD-686A-45A2-9CEA-E1A0A359ED54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4CF0A6-E882-4EB6-9A34-67F8138CD203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -714,6 +714,56 @@
   </si>
   <si>
     <t>App design and study</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Advised to use Influenzanet app directly rather than new app+integration
+2) Completed some of classification of group components related to roles and also question fetch from flat rendered items
+3) Started migration of all the app tointegrate with the Influenzanet app
+4) Every question should </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">be displayed in one screen i.e a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to question per screen. Needs to be clarified in the meeting</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -799,6 +849,21 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -814,21 +879,6 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -843,34 +893,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D18" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D18" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D19" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D19" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="6" xr3:uid="{1AEB8B07-63AC-4E5F-B5D7-DDB26374B386}" name="Date" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{A16789F0-4C4B-4A0A-AC1C-12937A234E71}" name="Phase" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{94CDE241-A8A3-4886-87C1-60BB038EEF8D}" name="Outline" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{8E2F684B-D9B1-4638-9E4C-1B47FC58B0B4}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{1AEB8B07-63AC-4E5F-B5D7-DDB26374B386}" name="Date" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A16789F0-4C4B-4A0A-AC1C-12937A234E71}" name="Phase" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{94CDE241-A8A3-4886-87C1-60BB038EEF8D}" name="Outline" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8E2F684B-D9B1-4638-9E4C-1B47FC58B0B4}" name="Comments" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A8CD2E07-0777-4479-9697-C502B276A704}" name="Table8" displayName="Table8" ref="A1:C6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A8CD2E07-0777-4479-9697-C502B276A704}" name="Table8" displayName="Table8" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C6" xr:uid="{6FF9E1DD-7A10-4235-8596-80FC9E7EFAB3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{53E311CE-6688-4AD7-A9F1-71D7B1497161}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{89A98BA3-5EEE-445F-A521-42228E721B59}" name="Queries" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00B1E2F2-FE81-453F-BB26-34D0B3887B3B}" name="Clarifications" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{53E311CE-6688-4AD7-A9F1-71D7B1497161}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{89A98BA3-5EEE-445F-A521-42228E721B59}" name="Queries" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00B1E2F2-FE81-453F-BB26-34D0B3887B3B}" name="Clarifications" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1173,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1438,6 +1488,20 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="86" x14ac:dyDescent="0.5">
+      <c r="A19" s="3">
+        <v>43986</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs(status) queries and status update
</commit_message>
<xml_diff>
--- a/documents/Status.xlsx
+++ b/documents/Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ananth\dart_projects\survey-engine.dart\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB31C33-CFBC-4A6C-8920-2497598F1690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB86B00-2CF9-41CE-9430-40F46598B074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E67059D-3E2D-46E3-97B8-C55C3B884939}"/>
   </bookViews>
   <sheets>
     <sheet name="Status(Summary)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -772,14 +772,22 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">App state management </t>
+  </si>
+  <si>
     <t xml:space="preserve">1) Migration of implemented code to Influenzanet app completed and Influenzanet app is used now for development
 2) Survey Single Item view is fetched from the data and almost all components are rendered with UX as per the web-client guideline
 3) Study of different architectures for app state management 
 4) Numerous trials using different variations of providers, inherited Widgets etc are done
 5) After a week of testing different state menagement techniques, started using ChangeNotifierProvider for survey page view and seperating model for survey single item
 6) After Q and A on 04/06/2020, decided to first implement a complete functioning app on a single page including rerendering functionality. Page breaks and other optimisations will be added at a later date 
-7) Present the findings and screenshots during syncup
+7) Presented the findings and screenshots during syncup
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Input data captured from textfields, formfields, radio buttons and checkboxes moved into app state
+2) Bug fixes during migration of elements from data stored in internal state to app state `Page Provider` 
+3) Started a simulation of rerendering and displaying survey items with preset (recorded) values on response change of each survey item </t>
   </si>
 </sst>
 </file>
@@ -909,8 +917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D20" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:D20" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{774D8131-A69C-4C93-A03C-6879BA904A1E}" name="Table6" displayName="Table6" ref="A1:D21" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D21" xr:uid="{D6280A21-F4EF-4765-A8E9-A4580F199CF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1239,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842C3C2D-255A-4DBA-8923-FAE573C0DD56}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1531,7 +1539,21 @@
         <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="86" x14ac:dyDescent="0.5">
+      <c r="A21" s="3">
+        <v>44007</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>